<commit_message>
pascal & single number
</commit_message>
<xml_diff>
--- a/Leetcode problem tracker.xlsx
+++ b/Leetcode problem tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Coding\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB08A642-216E-4108-9311-07F2B3289D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679329A5-0CC0-45AB-A5F6-F890827A6D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{365DB2E8-E54E-499E-9AF1-AA44A1C62DEA}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Algos" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Problems!$F$1:$F$133</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Problems!$F$1:$F$135</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -891,8 +891,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -949,6 +949,9 @@
       <c r="F3" s="2">
         <v>45468</v>
       </c>
+      <c r="G3" s="2">
+        <v>45549</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -1026,6 +1029,9 @@
       <c r="F7" s="2">
         <v>45480</v>
       </c>
+      <c r="G7" s="2">
+        <v>45549</v>
+      </c>
     </row>
     <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -1057,6 +1063,9 @@
       <c r="F9" s="2">
         <v>45480</v>
       </c>
+      <c r="G9" s="2">
+        <v>45555</v>
+      </c>
     </row>
     <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -1171,7 +1180,7 @@
         <v>45292</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>34</v>
       </c>
@@ -1190,8 +1199,11 @@
       <c r="F17" s="2">
         <v>45484</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" s="2">
+        <v>45560</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>35</v>
       </c>
@@ -1210,8 +1222,11 @@
       <c r="F18" s="2">
         <v>45468</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G18" s="2">
+        <v>45559</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>36</v>
       </c>
@@ -1222,7 +1237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>37</v>
       </c>
@@ -1233,7 +1248,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>41</v>
       </c>
@@ -1253,7 +1268,7 @@
         <v>45273</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>46</v>
       </c>
@@ -1264,7 +1279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>47</v>
       </c>
@@ -1275,7 +1290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>51</v>
       </c>
@@ -1286,7 +1301,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>52</v>
       </c>
@@ -1297,7 +1312,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>58</v>
       </c>
@@ -1316,8 +1331,11 @@
       <c r="F26" s="2">
         <v>45482</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G26" s="2">
+        <v>45552</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>61</v>
       </c>
@@ -1328,7 +1346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>66</v>
       </c>
@@ -1347,8 +1365,11 @@
       <c r="F28" s="2">
         <v>45470</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28" s="2">
+        <v>45549</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>67</v>
       </c>
@@ -1367,8 +1388,11 @@
       <c r="F29" s="2">
         <v>45480</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29" s="2">
+        <v>45555</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>69</v>
       </c>
@@ -1387,8 +1411,11 @@
       <c r="F30" s="2">
         <v>45468</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G30" s="2">
+        <v>45549</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>73</v>
       </c>
@@ -1408,7 +1435,7 @@
         <v>45361</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>74</v>
       </c>
@@ -1542,6 +1569,9 @@
       <c r="F40" s="2">
         <v>45484</v>
       </c>
+      <c r="G40" s="2">
+        <v>45560</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
@@ -1562,6 +1592,9 @@
       <c r="F41" s="2">
         <v>45484</v>
       </c>
+      <c r="G41" s="2">
+        <v>45560</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
@@ -1582,6 +1615,9 @@
       <c r="F42" s="2">
         <v>45468</v>
       </c>
+      <c r="G42" s="2">
+        <v>45552</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
@@ -1761,6 +1797,9 @@
       <c r="F52" s="2">
         <v>45469</v>
       </c>
+      <c r="G52" s="2">
+        <v>45552</v>
+      </c>
     </row>
     <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
@@ -1832,6 +1871,9 @@
       <c r="F56" s="2">
         <v>45480</v>
       </c>
+      <c r="G56" s="2">
+        <v>45559</v>
+      </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
@@ -1852,6 +1894,9 @@
       <c r="F57" s="2">
         <v>45469</v>
       </c>
+      <c r="G57" s="2">
+        <v>45559</v>
+      </c>
     </row>
     <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
@@ -1914,6 +1959,9 @@
       <c r="F61" s="2">
         <v>45469</v>
       </c>
+      <c r="G61" s="2">
+        <v>45552</v>
+      </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
@@ -1999,6 +2047,9 @@
       <c r="F66" s="2">
         <v>45468</v>
       </c>
+      <c r="G66" s="2">
+        <v>45552</v>
+      </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
@@ -2019,6 +2070,9 @@
       <c r="F67" s="2">
         <v>45469</v>
       </c>
+      <c r="G67" s="2">
+        <v>45559</v>
+      </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
@@ -2039,6 +2093,9 @@
       <c r="F68" s="2">
         <v>45469</v>
       </c>
+      <c r="G68" s="2">
+        <v>45560</v>
+      </c>
     </row>
     <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
@@ -2156,6 +2213,9 @@
       <c r="F74" s="2">
         <v>45480</v>
       </c>
+      <c r="G74" s="2">
+        <v>45549</v>
+      </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
@@ -2176,6 +2236,9 @@
       <c r="F75" s="2">
         <v>45480</v>
       </c>
+      <c r="G75" s="2">
+        <v>45549</v>
+      </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
@@ -2196,6 +2259,9 @@
       <c r="F76" s="2">
         <v>45481</v>
       </c>
+      <c r="G76" s="2">
+        <v>45549</v>
+      </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
@@ -2216,6 +2282,9 @@
       <c r="F77" s="2">
         <v>45481</v>
       </c>
+      <c r="G77" s="2">
+        <v>45549</v>
+      </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
@@ -2390,6 +2459,9 @@
       <c r="F86" s="2">
         <v>45493</v>
       </c>
+      <c r="G86" s="2">
+        <v>45549</v>
+      </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
@@ -2484,6 +2556,9 @@
       <c r="F91" s="2">
         <v>45468</v>
       </c>
+      <c r="G91" s="2">
+        <v>45549</v>
+      </c>
     </row>
     <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
@@ -2754,6 +2829,9 @@
       <c r="F106" s="2">
         <v>45468</v>
       </c>
+      <c r="G106" s="2">
+        <v>45549</v>
+      </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
@@ -2816,6 +2894,9 @@
       <c r="F110" s="2">
         <v>45482</v>
       </c>
+      <c r="G110" s="2">
+        <v>45560</v>
+      </c>
     </row>
     <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
@@ -2963,6 +3044,9 @@
       </c>
       <c r="F118" s="2">
         <v>45482</v>
+      </c>
+      <c r="G118" s="2">
+        <v>45560</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
@@ -3038,13 +3122,14 @@
         <v>131</v>
       </c>
     </row>
-    <row r="135" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="6:7" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="135" spans="6:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="F135" s="1" t="s">
         <v>127</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F1:F133" xr:uid="{3C0ADE24-140B-4EE6-A32B-01D05623BF43}">
+  <autoFilter ref="F1:F135" xr:uid="{3C0ADE24-140B-4EE6-A32B-01D05623BF43}">
     <filterColumn colId="0">
       <filters>
         <dateGroupItem year="2024" month="6" dateTimeGrouping="month"/>
@@ -3066,7 +3151,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3126,7 +3211,7 @@
         <v>45273</v>
       </c>
       <c r="F3" s="2">
-        <v>45468</v>
+        <v>45559</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -3143,7 +3228,7 @@
         <v>45273</v>
       </c>
       <c r="F4" s="2">
-        <v>45468</v>
+        <v>45559</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -3160,7 +3245,7 @@
         <v>45273</v>
       </c>
       <c r="F5" s="2">
-        <v>45468</v>
+        <v>45559</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>